<commit_message>
Register page added and updates done to code
</commit_message>
<xml_diff>
--- a/ParaBank/TestData/LoginData.xlsx
+++ b/ParaBank/TestData/LoginData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kritt\Desktop\GitHub\Selenium\ParaBank\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82177710-095A-4052-8646-D72829B37BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB66A9C-3192-4D47-BBCE-85385108A5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Register" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>userName</t>
   </si>
@@ -43,6 +44,51 @@
   </si>
   <si>
     <t>password12</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>ssn</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>52 King street</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>M5B 6A2</t>
   </si>
 </sst>
 </file>
@@ -362,7 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -399,4 +445,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53844496-C0C9-4526-BD0D-5FB7BF99E066}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>5556667777</v>
+      </c>
+      <c r="H2">
+        <v>88888888</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>